<commit_message>
added appnexus add functions along with other debug functions
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2935AC1F-F4C1-994D-B055-C0FF0F453CDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A2FE03-90C3-B54E-943C-126EBA6F6764}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus Add_Edit" sheetId="3" r:id="rId1"/>
@@ -1009,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2DFE33-156C-FF4B-85F5-5A363A8440C2}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1027,7 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
@@ -1150,7 +1150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3687A27C-9EB0-0D47-88CC-423BBFB909BB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1161,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
done with adding and edit functions
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A2FE03-90C3-B54E-943C-126EBA6F6764}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CFB779-51DE-6442-A5B9-666A27B330A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AppNexus Add_Edit" sheetId="3" r:id="rId1"/>
-    <sheet name="AppNexus Delete" sheetId="4" r:id="rId2"/>
-    <sheet name="TTD" sheetId="1" r:id="rId3"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
+    <sheet name="TTD" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Segment ID</t>
   </si>
@@ -120,28 +119,84 @@
     <t>Eyeota - US Media Source Solutions - Intent - Transaction Subcategory 2 - Medical Products - Diagnostics</t>
   </si>
   <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Chevrolet</t>
-  </si>
-  <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Chrysler</t>
-  </si>
-  <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Citroen</t>
-  </si>
-  <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Daihatsu</t>
-  </si>
-  <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Fiat</t>
-  </si>
-  <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Ford</t>
-  </si>
-  <si>
-    <t>Eyeota - UK Eyeota Auto Alliance - Intent - Auto Buyers - Car Makes - Hyundai</t>
-  </si>
-  <si>
-    <t>Required for Edit</t>
+    <t>Add: Required
+Edit: Required
+Delete: Optional</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Required if not public</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Edit: Not Required
+Delete: Not Required</t>
+    </r>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Delete: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required
+Retrieve ID: Required</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not Required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Edit: Optional
+Delete: Required</t>
+    </r>
+  </si>
+  <si>
+    <t>Not Required</t>
   </si>
 </sst>
 </file>
@@ -287,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,12 +525,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,11 +694,15 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1009,14 +1062,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2DFE33-156C-FF4B-85F5-5A363A8440C2}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -1051,36 +1112,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>6</v>
+    <row r="2" spans="1:10" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1147,125 +1208,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3687A27C-9EB0-0D47-88CC-423BBFB909BB}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>13529729</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>13529730</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>13529731</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>13529732</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>13529733</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>13529734</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>13529738</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
formatted input for Yahoo add
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362EFCE5-65F7-4043-BEE0-FA741888DCBF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4052444-8F5D-C248-B6B6-A52EDB0AEF8C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
     <sheet name="TTD" sheetId="1" r:id="rId2"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Segment ID</t>
   </si>
@@ -53,15 +54,6 @@
     <t>UK Kantar Media TGI &gt; Grocery Shopping &gt; Premium Range Purchasers</t>
   </si>
   <si>
-    <t>Healthy Food Buyers</t>
-  </si>
-  <si>
-    <t>Households that purchase Healthy food</t>
-  </si>
-  <si>
-    <t>Purchase Category &gt; Reach &gt; Healthy Food Buyers</t>
-  </si>
-  <si>
     <t>TV Channels Watched Live (Last 30 Days)</t>
   </si>
   <si>
@@ -69,15 +61,6 @@
   </si>
   <si>
     <t>Media &gt; TV And Film &gt; TV Channels Watched Live (Last 30 Days)</t>
-  </si>
-  <si>
-    <t>Good Food</t>
-  </si>
-  <si>
-    <t>Users that watch live the TV channel Good Food</t>
-  </si>
-  <si>
-    <t>Media &gt; TV And Film &gt; TV Channels Watched Live (Last 30 Days) &gt; Good Food</t>
   </si>
   <si>
     <t>Parent Segment ID</t>
@@ -202,6 +185,30 @@
 Delete: Not Required
 Retrieve: Not Required</t>
     </r>
+  </si>
+  <si>
+    <t>UK Kantar Media TGI - Grocery Shopping - Premium Range Purchasers</t>
+  </si>
+  <si>
+    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Rich People</t>
+  </si>
+  <si>
+    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People</t>
+  </si>
+  <si>
+    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People - Even Poorer People</t>
+  </si>
+  <si>
+    <t>Just random segment 4444</t>
+  </si>
+  <si>
+    <t>Just random segment 1111</t>
+  </si>
+  <si>
+    <t>Just random segment 2222</t>
+  </si>
+  <si>
+    <t>Just random segment 3333</t>
   </si>
 </sst>
 </file>
@@ -1072,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2DFE33-156C-FF4B-85F5-5A363A8440C2}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1095,63 +1102,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="9"/>
     </row>
@@ -1160,7 +1167,7 @@
         <v>-2147403569</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1172,16 +1179,13 @@
         <v>1706</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>4299</v>
-      </c>
-      <c r="J3">
-        <v>1832</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1189,7 +1193,7 @@
         <v>-2147401991</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1201,7 +1205,7 @@
         <v>1706</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -1220,41 +1224,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>31804</v>
+      </c>
+      <c r="B3">
+        <v>4427</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>32048</v>
+      </c>
+      <c r="B4">
+        <v>32039</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27763304-9429-BE47-B12E-8F44F8D57B16}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1264,124 +1372,52 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>31804</v>
-      </c>
-      <c r="B3">
-        <v>4427</v>
+        <v>4444</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>31868</v>
-      </c>
-      <c r="B4">
-        <v>7807</v>
+        <v>1111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>32048</v>
-      </c>
-      <c r="B5">
-        <v>32039</v>
+        <v>2222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>32069</v>
-      </c>
-      <c r="B6">
-        <v>32048</v>
+        <v>3333</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test data to TTD upload worksheet
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4052444-8F5D-C248-B6B6-A52EDB0AEF8C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D234E19-69AA-6E41-B4A7-636729EBDAC5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Segment ID</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Just random segment 3333</t>
+  </si>
+  <si>
+    <t>taxoapitest</t>
   </si>
 </sst>
 </file>
@@ -1226,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1289,51 +1292,51 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>31804</v>
-      </c>
-      <c r="B3">
-        <v>4427</v>
+        <v>32048</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" s="1">
-        <v>1.5</v>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>32048</v>
+        <v>31804</v>
       </c>
       <c r="B4">
-        <v>32039</v>
+        <v>31804</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" s="1">
+        <v>1.5</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27763304-9429-BE47-B12E-8F44F8D57B16}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Yahoo refresh taxo function is up for testing
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D234E19-69AA-6E41-B4A7-636729EBDAC5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF6B935-0BB9-AB47-A2AF-238068074798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="1300" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
@@ -1229,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1348,11 +1348,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27763304-9429-BE47-B12E-8F44F8D57B16}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="77.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
added data source in add segments fuction for AAM
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF6B935-0BB9-AB47-A2AF-238068074798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="1300" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="1305" windowWidth="28035" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
-    <sheet name="TTD" sheetId="1" r:id="rId2"/>
-    <sheet name="Yahoo" sheetId="4" r:id="rId3"/>
+    <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
+    <sheet name="TTD" sheetId="1" r:id="rId3"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t>Segment ID</t>
   </si>
@@ -103,11 +98,58 @@
   </si>
   <si>
     <t>Not Required</t>
+  </si>
+  <si>
+    <t>UK Kantar Media TGI - Grocery Shopping - Premium Range Purchasers</t>
+  </si>
+  <si>
+    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Rich People</t>
+  </si>
+  <si>
+    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People</t>
+  </si>
+  <si>
+    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People - Even Poorer People</t>
+  </si>
+  <si>
+    <t>Just random segment 4444</t>
+  </si>
+  <si>
+    <t>Just random segment 1111</t>
+  </si>
+  <si>
+    <t>Just random segment 2222</t>
+  </si>
+  <si>
+    <t>Just random segment 3333</t>
+  </si>
+  <si>
+    <t>taxoapitest</t>
+  </si>
+  <si>
+    <t>Segment Status</t>
+  </si>
+  <si>
+    <t>Data Source ID</t>
+  </si>
+  <si>
+    <t>Data Source Name</t>
+  </si>
+  <si>
+    <t>Segments and Overlap Price</t>
+  </si>
+  <si>
+    <t>Segments and Overlap UoM</t>
+  </si>
+  <si>
+    <t>Modeling Price</t>
+  </si>
+  <si>
+    <t>Modeling UoM</t>
   </si>
   <si>
     <t>Add: Required
 Edit: Required
-Delete: Not Required
 Retrieve: Required</t>
   </si>
   <si>
@@ -135,26 +177,17 @@
       </rPr>
       <t xml:space="preserve">
 Edit: Optional
-Delete: Required
 Retrieve: Not Required</t>
     </r>
   </si>
   <si>
     <t>Add: Required
 Edit: Required
-Delete: Not Required
-Retrieve: Not Required</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
-Delete: Optional
 Retrieve: Not Required</t>
   </si>
   <si>
     <t>Add: Required
 Edit: Not Required
-Delete: Not Required
 Retrieve: Not Required</t>
   </si>
   <si>
@@ -182,46 +215,33 @@
       </rPr>
       <t xml:space="preserve">
 Edit: Not Required
-Delete: Not Required
 Retrieve: Not Required</t>
     </r>
   </si>
   <si>
-    <t>UK Kantar Media TGI - Grocery Shopping - Premium Range Purchasers</t>
-  </si>
-  <si>
-    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Rich People</t>
-  </si>
-  <si>
-    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People</t>
-  </si>
-  <si>
-    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People - Even Poorer People</t>
-  </si>
-  <si>
-    <t>Just random segment 4444</t>
-  </si>
-  <si>
-    <t>Just random segment 1111</t>
-  </si>
-  <si>
-    <t>Just random segment 2222</t>
-  </si>
-  <si>
-    <t>Just random segment 3333</t>
-  </si>
-  <si>
-    <t>taxoapitest</t>
+    <t>Add: Required</t>
+  </si>
+  <si>
+    <t>Activation Price</t>
+  </si>
+  <si>
+    <t>Activation UoM</t>
+  </si>
+  <si>
+    <t>Add: Optional</t>
+  </si>
+  <si>
+    <t>test20181028</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,6 +376,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -544,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -659,6 +684,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -704,7 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -724,6 +764,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -826,7 +869,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -878,7 +921,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1072,35 +1115,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2DFE33-156C-FF4B-85F5-5A363A8440C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.375" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.625" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.375" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" customWidth="1"/>
+    <col min="10" max="10" width="23.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1132,40 +1175,40 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="68.099999999999994" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="B3">
         <v>-2147403569</v>
       </c>
@@ -1191,7 +1234,7 @@
         <v>4299</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="B4">
         <v>-2147401991</v>
       </c>
@@ -1226,19 +1269,132 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="66.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="47.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1264,7 +1420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1290,12 +1446,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>32048</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1313,7 +1469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>31804</v>
       </c>
@@ -1344,21 +1500,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27763304-9429-BE47-B12E-8F44F8D57B16}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="77.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1369,7 +1525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1380,48 +1536,48 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>4444</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1111</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2222</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>3333</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
able to add trait folders now
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1080E7-BD19-D14F-A675-596D54E54F91}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="1305" windowWidth="28035" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="5560" yWindow="1300" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>Segment ID</t>
   </si>
@@ -233,15 +239,42 @@
   <si>
     <t>test20181028</t>
   </si>
+  <si>
+    <t>Data Feed Description</t>
+  </si>
+  <si>
+    <t>Add: Optional if data source exists</t>
+  </si>
+  <si>
+    <t>Test on 20181028</t>
+  </si>
+  <si>
+    <t>Not Required (default FIXED)</t>
+  </si>
+  <si>
+    <t>Add: Optional (FIXED or CPM)</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Trait Folder Path</t>
+  </si>
+  <si>
+    <t>/All Traits/TEST20181029</t>
+  </si>
+  <si>
+    <t>/All Traits/TEST20181029/TEST</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,6 +413,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -869,7 +903,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -921,7 +955,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1115,35 +1149,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="A2:J2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.375" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.875" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="68.099999999999994" customHeight="1">
+    <row r="2" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1208,7 +1242,7 @@
       </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-2147403569</v>
       </c>
@@ -1234,7 +1268,7 @@
         <v>4299</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-2147401991</v>
       </c>
@@ -1269,30 +1303,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1306,31 +1342,37 @@
         <v>36</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
@@ -1343,37 +1385,63 @@
       <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>48</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="F3" t="s">
+      <c r="N2" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
         <v>52</v>
       </c>
-      <c r="G3">
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3">
         <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1382,19 +1450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="66.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="47.25">
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1446,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>32048</v>
       </c>
@@ -1469,7 +1537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>31804</v>
       </c>
@@ -1501,20 +1569,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="77.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1536,7 +1604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4444</v>
       </c>
@@ -1547,7 +1615,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1111</v>
       </c>
@@ -1558,7 +1626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2222</v>
       </c>
@@ -1569,7 +1637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3333</v>
       </c>

</xml_diff>

<commit_message>
adobe add segments function is working
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1080E7-BD19-D14F-A675-596D54E54F91}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA06644-C3B4-6E48-9920-BEBAC5004756}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="1300" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Segment ID</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Add: Optional</t>
   </si>
   <si>
-    <t>test20181028</t>
-  </si>
-  <si>
     <t>Data Feed Description</t>
   </si>
   <si>
@@ -261,10 +258,28 @@
     <t>Trait Folder Path</t>
   </si>
   <si>
-    <t>/All Traits/TEST20181029</t>
-  </si>
-  <si>
-    <t>/All Traits/TEST20181029/TEST</t>
+    <t>/All Traits/TEST20181030/TEST</t>
+  </si>
+  <si>
+    <t>/All Traits/TEST20181030</t>
+  </si>
+  <si>
+    <t>Segment Lifetime</t>
+  </si>
+  <si>
+    <t>Test Segment 1</t>
+  </si>
+  <si>
+    <t>Test Segment 2</t>
+  </si>
+  <si>
+    <t>Test Description 1</t>
+  </si>
+  <si>
+    <t>Test Description 2</t>
+  </si>
+  <si>
+    <t>test20181030</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,19 +1331,19 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1342,37 +1357,40 @@
         <v>36</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="I1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
@@ -1388,60 +1406,84 @@
       <c r="E2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4">
         <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added segment loads report for AppNexus
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA06644-C3B4-6E48-9920-BEBAC5004756}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C41DADA-6765-1B46-B32F-A6B7D5514610}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1300" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>Segment ID</t>
   </si>
@@ -281,6 +281,28 @@
   <si>
     <t>test20181030</t>
   </si>
+  <si>
+    <t>Report Start Date</t>
+  </si>
+  <si>
+    <t>Report End Date</t>
+  </si>
+  <si>
+    <t>Required for Getting Report</t>
+  </si>
+  <si>
+    <t>Exclusive!!
+Required for Getting Report</t>
+  </si>
+  <si>
+    <t>Report Email</t>
+  </si>
+  <si>
+    <t>asoh@eyeota.com</t>
+  </si>
+  <si>
+    <t>asoh@eyeota.com, ykoh@eyeota.com</t>
+  </si>
 </sst>
 </file>
 
@@ -289,7 +311,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -429,6 +451,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -749,7 +779,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -792,8 +822,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -811,14 +842,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -852,6 +885,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1172,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,9 +1224,10 @@
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.83203125" customWidth="1"/>
+    <col min="11" max="12" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1223,8 +1258,17 @@
       <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1255,9 +1299,17 @@
       <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-2147403569</v>
       </c>
@@ -1282,8 +1334,17 @@
       <c r="I3">
         <v>4299</v>
       </c>
+      <c r="K3" s="11">
+        <v>43405</v>
+      </c>
+      <c r="L3" s="11">
+        <v>43411</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-2147401991</v>
       </c>
@@ -1311,8 +1372,21 @@
       <c r="J4">
         <v>1832</v>
       </c>
+      <c r="K4" s="11">
+        <v>43412</v>
+      </c>
+      <c r="L4" s="11">
+        <v>43413</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M3" r:id="rId1" display="asoh@eyeota.com" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1321,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1344,49 +1418,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished add segments function for Adform
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C41DADA-6765-1B46-B32F-A6B7D5514610}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1846305F-355A-314F-8FFD-CC12BE41D7DA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
-    <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
-    <sheet name="TTD" sheetId="1" r:id="rId3"/>
-    <sheet name="Yahoo" sheetId="4" r:id="rId4"/>
+    <sheet name="Adform" sheetId="6" r:id="rId1"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId2"/>
+    <sheet name="Adobe AAM" sheetId="5" r:id="rId3"/>
+    <sheet name="TTD" sheetId="1" r:id="rId4"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="82">
   <si>
     <t>Segment ID</t>
   </si>
@@ -303,6 +304,32 @@
   <si>
     <t>asoh@eyeota.com, ykoh@eyeota.com</t>
   </si>
+  <si>
+    <t>Ref ID</t>
+  </si>
+  <si>
+    <t>Fee</t>
+  </si>
+  <si>
+    <t>TTL</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Add: Required
+Values: global, apac
+Defaulted to global</t>
+  </si>
+  <si>
+    <t>apac</t>
+  </si>
+  <si>
+    <t>TEST 20181108 - Child Segment 20181108008</t>
+  </si>
+  <si>
+    <t>TEST 20181108 - TEST 20181108 Layer 1 - Child Segment 20181108007</t>
+  </si>
 </sst>
 </file>
 
@@ -311,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -460,6 +487,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -648,7 +683,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -778,6 +813,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -824,7 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -850,6 +898,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1205,11 +1262,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20181108007</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20181108008</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,7 +1537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -1565,7 +1711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1684,7 +1830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>

<commit_message>
sorted tabs for uploadtemplate
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1846305F-355A-314F-8FFD-CC12BE41D7DA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B176B0A-5FC0-7241-B916-24D4EE003414}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
-    <sheet name="AppNexus" sheetId="3" r:id="rId2"/>
-    <sheet name="Adobe AAM" sheetId="5" r:id="rId3"/>
+    <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId3"/>
     <sheet name="TTD" sheetId="1" r:id="rId4"/>
     <sheet name="Yahoo" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -1265,7 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1351,6 +1351,180 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -1537,180 +1711,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4">
-        <v>90</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>

</xml_diff>

<commit_message>
edited Adobe AAM to print out error message for add trait
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B176B0A-5FC0-7241-B916-24D4EE003414}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40CDF13-8268-1444-8C34-A922513B4243}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,12 +274,6 @@
     <t>Test Segment 2</t>
   </si>
   <si>
-    <t>Test Description 1</t>
-  </si>
-  <si>
-    <t>Test Description 2</t>
-  </si>
-  <si>
     <t>test20181030</t>
   </si>
   <si>
@@ -329,6 +323,12 @@
   </si>
   <si>
     <t>TEST 20181108 - TEST 20181108 Layer 1 - Child Segment 20181108007</t>
+  </si>
+  <si>
+    <t>Test Description 1</t>
+  </si>
+  <si>
+    <t>Test Description 2</t>
   </si>
 </sst>
 </file>
@@ -1279,19 +1279,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1302,7 +1302,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>48</v>
@@ -1316,10 +1316,10 @@
         <v>20181108007</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1333,10 +1333,10 @@
         <v>20181108008</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1355,7 +1355,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1475,7 +1475,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>90</v>
@@ -1484,7 +1484,7 @@
         <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
         <v>54</v>
@@ -1504,7 +1504,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E4">
         <v>90</v>
@@ -1513,7 +1513,7 @@
         <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1579,13 +1579,13 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -1620,13 +1620,13 @@
         <v>47</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1661,7 +1661,7 @@
         <v>43411</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1699,7 +1699,7 @@
         <v>43413</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to debug adobe aam create trait folder
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40CDF13-8268-1444-8C34-A922513B4243}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE817648-13C8-9041-9D78-00B606028A4F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -114,12 +114,6 @@
   </si>
   <si>
     <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People</t>
-  </si>
-  <si>
-    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People - Even Poorer People</t>
-  </si>
-  <si>
-    <t>Just random segment 4444</t>
   </si>
   <si>
     <t>Just random segment 1111</t>
@@ -329,6 +323,12 @@
   </si>
   <si>
     <t>Test Description 2</t>
+  </si>
+  <si>
+    <t>This is simply a test</t>
+  </si>
+  <si>
+    <t>Test 5555</t>
   </si>
 </sst>
 </file>
@@ -1279,36 +1279,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1316,10 +1316,10 @@
         <v>20181108007</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1333,10 +1333,10 @@
         <v>20181108008</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1354,7 +1354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1387,40 +1387,40 @@
         <v>14</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="N1" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -1428,66 +1428,66 @@
         <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3">
         <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1496,24 +1496,24 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4">
         <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1579,54 +1579,54 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="K2" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1661,7 +1661,7 @@
         <v>43411</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1699,7 +1699,7 @@
         <v>43413</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +1781,7 @@
         <v>32048</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1834,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1868,46 +1868,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4444</v>
+        <v>1111</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1111</v>
+        <v>2222</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2222</v>
+        <v>3333</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3333</v>
+        <v>5555</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed oath refresh segments
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE817648-13C8-9041-9D78-00B606028A4F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECF989F-84F0-F24E-B3E4-0BC96FBE313A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="TTD" sheetId="1" r:id="rId4"/>
     <sheet name="Yahoo" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
   <si>
     <t>Segment ID</t>
   </si>
@@ -253,16 +253,7 @@
     <t>Trait Folder Path</t>
   </si>
   <si>
-    <t>/All Traits/TEST20181030/TEST</t>
-  </si>
-  <si>
-    <t>/All Traits/TEST20181030</t>
-  </si>
-  <si>
     <t>Segment Lifetime</t>
-  </si>
-  <si>
-    <t>Test Segment 1</t>
   </si>
   <si>
     <t>Test Segment 2</t>
@@ -288,9 +279,6 @@
   </si>
   <si>
     <t>asoh@eyeota.com</t>
-  </si>
-  <si>
-    <t>asoh@eyeota.com, ykoh@eyeota.com</t>
   </si>
   <si>
     <t>Ref ID</t>
@@ -329,6 +317,12 @@
   </si>
   <si>
     <t>Test 5555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Segment 1 Test Segment 1 Test Segment 1 Test Segment 1 Test </t>
+  </si>
+  <si>
+    <t>/All Traits/TEST20181112/TEST</t>
   </si>
 </sst>
 </file>
@@ -1279,19 +1273,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1302,7 +1296,7 @@
         <v>46</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>46</v>
@@ -1316,10 +1310,10 @@
         <v>20181108007</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1333,10 +1327,10 @@
         <v>20181108008</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1354,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1384,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>56</v>
@@ -1472,19 +1466,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E3">
         <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
         <v>52</v>
@@ -1501,19 +1495,19 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E4">
         <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1529,7 +1523,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1579,13 +1573,13 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -1620,13 +1614,13 @@
         <v>45</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1661,7 +1655,7 @@
         <v>43411</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1699,12 +1693,12 @@
         <v>43413</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" display="asoh@eyeota.com" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
     <hyperlink ref="M4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1834,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1904,10 +1898,10 @@
         <v>5555</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data usage report for AppNexus
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECF989F-84F0-F24E-B3E4-0BC96FBE313A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB00D4B-05CC-EF47-95F0-D011B703CE31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Segment ID</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Member ID</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -104,34 +101,19 @@
     <t>Eyeota - US Media Source Solutions - Intent - Transaction Subcategory 2 - Medical Products - Diagnostics</t>
   </si>
   <si>
-    <t>Not Required</t>
-  </si>
-  <si>
     <t>UK Kantar Media TGI - Grocery Shopping - Premium Range Purchasers</t>
   </si>
   <si>
     <t>Purchase Category - Reach - Healthy Food Buyers - Damn Rich People</t>
   </si>
   <si>
-    <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People</t>
-  </si>
-  <si>
     <t>Just random segment 1111</t>
   </si>
   <si>
     <t>Just random segment 2222</t>
   </si>
   <si>
-    <t>Just random segment 3333</t>
-  </si>
-  <si>
     <t>taxoapitest</t>
-  </si>
-  <si>
-    <t>Segment Status</t>
-  </si>
-  <si>
-    <t>Data Source ID</t>
   </si>
   <si>
     <t>Data Source Name</t>
@@ -271,10 +253,6 @@
     <t>Required for Getting Report</t>
   </si>
   <si>
-    <t>Exclusive!!
-Required for Getting Report</t>
-  </si>
-  <si>
     <t>Report Email</t>
   </si>
   <si>
@@ -313,16 +291,37 @@
     <t>Test Description 2</t>
   </si>
   <si>
-    <t>This is simply a test</t>
-  </si>
-  <si>
-    <t>Test 5555</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test Segment 1 Test Segment 1 Test Segment 1 Test Segment 1 Test </t>
   </si>
   <si>
     <t>/All Traits/TEST20181112/TEST</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exclusive!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Required for Getting Report</t>
+    </r>
+  </si>
+  <si>
+    <t>asoh@eyeota.com,dataops@eyeota.com</t>
   </si>
 </sst>
 </file>
@@ -866,29 +865,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
@@ -898,9 +879,34 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1257,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,51 +1275,65 @@
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20181108007</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1321,22 +1341,34 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="3">
+        <v>43405</v>
+      </c>
+      <c r="G3" s="3">
+        <v>43412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20181108008</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43412</v>
+      </c>
+      <c r="G4" s="3">
+        <v>43413</v>
       </c>
     </row>
   </sheetData>
@@ -1346,170 +1378,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4">
-        <v>90</v>
-      </c>
-      <c r="F4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4">
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
@@ -1520,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,102 +1544,95 @@
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" customWidth="1"/>
-    <col min="11" max="12" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-2147403569</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1636,34 +1640,31 @@
       <c r="E3">
         <v>129600</v>
       </c>
-      <c r="F3">
-        <v>1706</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="b">
+      <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="H3">
         <v>4299</v>
       </c>
-      <c r="K3" s="11">
+      <c r="J3" s="3">
         <v>43405</v>
       </c>
-      <c r="L3" s="11">
-        <v>43411</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K3" s="3">
+        <v>43412</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-2147401991</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1671,35 +1672,32 @@
       <c r="E4">
         <v>129600</v>
       </c>
-      <c r="F4">
-        <v>1706</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="b">
+      <c r="G4" t="b">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>4299</v>
+      </c>
       <c r="I4">
-        <v>4299</v>
-      </c>
-      <c r="J4">
         <v>1832</v>
       </c>
-      <c r="K4" s="11">
+      <c r="J4" s="3">
         <v>43412</v>
       </c>
-      <c r="L4" s="11">
+      <c r="K4" s="3">
         <v>43413</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>65</v>
+      <c r="L4" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
-    <hyperlink ref="M4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
+    <hyperlink ref="L4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1710,7 +1708,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1719,54 +1717,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1775,7 +1773,7 @@
         <v>32048</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1826,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1839,24 +1837,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1865,10 +1863,10 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1876,32 +1874,10 @@
         <v>2222</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3333</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5555</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added description for appnexus segment, and data segment type id for segment billing
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB00D4B-05CC-EF47-95F0-D011B703CE31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CA9F92-0819-7447-9599-7694D45F5B38}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>Segment ID</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>asoh@eyeota.com,dataops@eyeota.com</t>
+  </si>
+  <si>
+    <t>Data Segment Type ID</t>
   </si>
 </sst>
 </file>
@@ -1531,27 +1534,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" customWidth="1"/>
-    <col min="10" max="11" width="14.33203125" customWidth="1"/>
+    <col min="3" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" customWidth="1"/>
+    <col min="12" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1562,34 +1565,40 @@
         <v>1</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -1609,95 +1618,113 @@
         <v>37</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-2147403569</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>129600</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="b">
+      <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
         <v>4299</v>
       </c>
-      <c r="J3" s="3">
+      <c r="L3" s="3">
         <v>43405</v>
       </c>
-      <c r="K3" s="3">
+      <c r="M3" s="3">
         <v>43412</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-2147401991</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>129600</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="b">
+      <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
+        <v>200</v>
+      </c>
+      <c r="J4">
         <v>4299</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>1832</v>
       </c>
-      <c r="J4" s="3">
+      <c r="L4" s="3">
         <v>43412</v>
       </c>
-      <c r="K4" s="3">
+      <c r="M4" s="3">
         <v>43413</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
-    <hyperlink ref="L4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
+    <hyperlink ref="N3" r:id="rId1" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added two more fields to Yahoo upload file
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CA9F92-0819-7447-9599-7694D45F5B38}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8269BC-3881-DD42-95DF-9373157AF070}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
   <si>
     <t>Segment ID</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>Data Segment Type ID</t>
+  </si>
+  <si>
+    <t>Segment Key</t>
+  </si>
+  <si>
+    <t>Eyeota Segment Name</t>
   </si>
 </sst>
 </file>
@@ -823,7 +829,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -867,8 +873,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -910,8 +917,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -950,6 +958,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 3" xfId="43" xr:uid="{5B8E2594-CA1F-5844-9172-955DD5C344DB}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1536,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1851,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1863,7 +1872,7 @@
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1873,8 +1882,14 @@
       <c r="C1" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="D1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -1884,8 +1899,14 @@
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1111</v>
       </c>
@@ -1896,7 +1917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2222</v>
       </c>

</xml_diff>

<commit_message>
fixed appnexus report to retrieve from interface
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8269BC-3881-DD42-95DF-9373157AF070}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE16A80-AE2A-AF40-B18F-125CABB323CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Segment ID</t>
   </si>
@@ -253,12 +253,6 @@
     <t>Required for Getting Report</t>
   </si>
   <si>
-    <t>Report Email</t>
-  </si>
-  <si>
-    <t>asoh@eyeota.com</t>
-  </si>
-  <si>
     <t>Ref ID</t>
   </si>
   <si>
@@ -321,9 +315,6 @@
     </r>
   </si>
   <si>
-    <t>asoh@eyeota.com,dataops@eyeota.com</t>
-  </si>
-  <si>
     <t>Data Segment Type ID</t>
   </si>
   <si>
@@ -340,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,14 +471,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -829,7 +812,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -872,24 +855,22 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -919,7 +900,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -953,12 +934,11 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 3" xfId="43" xr:uid="{5B8E2594-CA1F-5844-9172-955DD5C344DB}"/>
+    <cellStyle name="Normal 2 3" xfId="42" xr:uid="{5B8E2594-CA1F-5844-9172-955DD5C344DB}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1292,49 +1272,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>71</v>
+      <c r="G2" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1342,10 +1322,10 @@
         <v>20181108007</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1365,10 +1345,10 @@
         <v>20181108008</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1450,55 +1430,55 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
@@ -1521,13 +1501,13 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4">
         <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -1543,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1563,95 +1543,89 @@
     <col min="12" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M2" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-2147403569</v>
       </c>
@@ -1659,7 +1633,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1685,11 +1659,8 @@
       <c r="M3" s="3">
         <v>43412</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-2147401991</v>
       </c>
@@ -1697,7 +1668,7 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1726,15 +1697,8 @@
       <c r="M4" s="3">
         <v>43413</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>58</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" xr:uid="{F48E54AA-C723-9443-BB46-435CC1B9D816}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{D022A140-4761-9C45-9070-2C8470824D5E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1753,54 +1717,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1862,7 +1826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1873,36 +1837,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>75</v>
+      <c r="D1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added functions to get data usage report from all platforms with such report
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE16A80-AE2A-AF40-B18F-125CABB323CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7650D0-EBAF-F645-AB05-B83818953732}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,13 +18,14 @@
     <sheet name="AppNexus" sheetId="3" r:id="rId3"/>
     <sheet name="TTD" sheetId="1" r:id="rId4"/>
     <sheet name="Yahoo" sheetId="4" r:id="rId5"/>
+    <sheet name="All Report Platforms" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>Segment ID</t>
   </si>
@@ -857,7 +858,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -899,6 +900,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1526,7 +1530,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1895,4 +1899,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACD0D70-707D-6848-808A-BFBD2B8DA8BA}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>43405</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43412</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added adobe aam get subscribers contacts function
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7650D0-EBAF-F645-AB05-B83818953732}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3ECA53-0ABB-A040-B3C0-87215735D584}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1280" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1340" windowWidth="31860" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>Segment ID</t>
   </si>
@@ -266,18 +266,10 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Add: Required
-Values: global, apac
-Defaulted to global</t>
-  </si>
-  <si>
     <t>apac</t>
   </si>
   <si>
     <t>TEST 20181108 - Child Segment 20181108008</t>
-  </si>
-  <si>
-    <t>TEST 20181108 - TEST 20181108 Layer 1 - Child Segment 20181108007</t>
   </si>
   <si>
     <t>Test Description 1</t>
@@ -323,6 +315,38 @@
   </si>
   <si>
     <t>Eyeota Segment Name</t>
+  </si>
+  <si>
+    <t>Add: Not required
+Edit: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Values: global, apac
+Defaulted to global</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>TEST 20181108 - TEST 20181108 Layer 2 - Child Segment 20181108007</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>inactive</t>
   </si>
 </sst>
 </file>
@@ -858,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -903,6 +927,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1259,111 +1287,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>40</v>
+    <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
+        <v>1359266</v>
+      </c>
+      <c r="B3">
+        <v>20181108007</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>20181108007</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="3">
         <v>43405</v>
       </c>
-      <c r="G3" s="3">
+      <c r="I3" s="3">
         <v>43412</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <v>1359267</v>
+      </c>
+      <c r="B4">
         <v>20181108008</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="3">
         <v>43412</v>
       </c>
-      <c r="G4" s="3">
+      <c r="I4" s="3">
         <v>43413</v>
       </c>
     </row>
@@ -1374,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1387,15 +1441,16 @@
     <col min="3" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1415,25 +1470,28 @@
         <v>44</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
@@ -1455,34 +1513,37 @@
       <c r="G2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
@@ -1490,33 +1551,39 @@
       <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4">
         <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
@@ -1529,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -1573,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>17</v>
@@ -1626,7 +1693,7 @@
         <v>56</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1637,7 +1704,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1672,7 +1739,7 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1851,10 +1918,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1924,7 +1991,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
edited edit segments function in AppNexus to be able to change code (segment key)
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3ECA53-0ABB-A040-B3C0-87215735D584}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD330656-6129-8049-B50B-7D3E7F8BA44A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1340" windowWidth="31860" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1340" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -94,12 +94,6 @@
   </si>
   <si>
     <t>Buyer Member ID</t>
-  </si>
-  <si>
-    <t>Eyeota - US Media Source Solutions - Intent - Transaction Subcategory 2 - Luggage</t>
-  </si>
-  <si>
-    <t>Eyeota - US Media Source Solutions - Intent - Transaction Subcategory 2 - Medical Products - Diagnostics</t>
   </si>
   <si>
     <t>UK Kantar Media TGI - Grocery Shopping - Premium Range Purchasers</t>
@@ -347,6 +341,12 @@
   </si>
   <si>
     <t>inactive</t>
+  </si>
+  <si>
+    <t>Test Segment Name 30 Nov 2018 1</t>
+  </si>
+  <si>
+    <t>Test Segment Name 30 Nov 2018 2</t>
   </si>
 </sst>
 </file>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,71 +1310,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="21">
-        <v>1359266</v>
-      </c>
+      <c r="A3" s="21"/>
       <c r="B3">
-        <v>20181108007</v>
+        <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1383,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1393,17 +1391,15 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
-        <v>1359267</v>
-      </c>
+      <c r="A4" s="21"/>
       <c r="B4">
-        <v>20181108008</v>
+        <v>20181130001</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1412,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H4" s="3">
         <v>43412</v>
@@ -1458,101 +1454,101 @@
         <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="J2" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1561,27 +1557,27 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4">
         <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1596,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1640,7 +1636,7 @@
         <v>16</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>17</v>
@@ -1649,62 +1645,65 @@
         <v>22</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="I2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="L2" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>15662758</v>
+      </c>
       <c r="B3">
-        <v>-2147403569</v>
+        <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1732,14 +1731,17 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>15662759</v>
+      </c>
       <c r="B4">
-        <v>-2147401991</v>
+        <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1751,7 +1753,7 @@
         <v>18</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>200</v>
@@ -1844,7 +1846,7 @@
         <v>32048</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1918,10 +1920,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1946,10 +1948,10 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1957,10 +1959,10 @@
         <v>2222</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1980,18 +1982,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added additional field for Yahoo tab for Private Buyer ID
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,27 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC512C26-5F4D-5642-9402-100F5C049D43}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2173B-612D-844A-91A3-1D4497F8630F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1340" windowWidth="31860" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="980" windowWidth="31860" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
     <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
     <sheet name="AppNexus" sheetId="3" r:id="rId3"/>
-    <sheet name="TTD" sheetId="1" r:id="rId4"/>
-    <sheet name="Yahoo" sheetId="4" r:id="rId5"/>
-    <sheet name="All Report Platforms" sheetId="7" r:id="rId6"/>
+    <sheet name="MediaMath" sheetId="8" r:id="rId4"/>
+    <sheet name="TTD" sheetId="1" r:id="rId5"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId6"/>
+    <sheet name="All Report Platforms" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
   <si>
     <t>Segment ID</t>
   </si>
@@ -187,9 +188,6 @@
     <t>Add: Optional if data source exists</t>
   </si>
   <si>
-    <t>Test on 20181028</t>
-  </si>
-  <si>
     <t>Not Required (default FIXED)</t>
   </si>
   <si>
@@ -205,12 +203,6 @@
     <t>Segment Lifetime</t>
   </si>
   <si>
-    <t>Test Segment 2</t>
-  </si>
-  <si>
-    <t>test20181030</t>
-  </si>
-  <si>
     <t>Report Start Date</t>
   </si>
   <si>
@@ -235,9 +227,6 @@
     <t>apac</t>
   </si>
   <si>
-    <t>TEST 20181108 - Child Segment 20181108008</t>
-  </si>
-  <si>
     <t>Test Description 1</t>
   </si>
   <si>
@@ -245,9 +234,6 @@
   </si>
   <si>
     <t xml:space="preserve">Test Segment 1 Test Segment 1 Test Segment 1 Test Segment 1 Test </t>
-  </si>
-  <si>
-    <t>/All Traits/TEST20181112/TEST</t>
   </si>
   <si>
     <r>
@@ -301,9 +287,6 @@
   </si>
   <si>
     <t>Private</t>
-  </si>
-  <si>
-    <t>Public</t>
   </si>
   <si>
     <t>TEST 20181108 - TEST 20181108 Layer 2 - Child Segment 20181108007</t>
@@ -348,6 +331,76 @@
 Retrieve: Not Required</t>
     </r>
   </si>
+  <si>
+    <t>test20181207</t>
+  </si>
+  <si>
+    <t>Test on 20181207</t>
+  </si>
+  <si>
+    <t>/All Traits/3rd-Party Data/test20181207/TEST</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add: Required
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>Note the folder after "All Traits/3rd-Party Data" should follow the Data Source Name</t>
+    </r>
+  </si>
+  <si>
+    <t>uniques</t>
+  </si>
+  <si>
+    <t>Wholesale CPM</t>
+  </si>
+  <si>
+    <t>Retail CPM</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions - Business Owners</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions - C-Suite / C-Level</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions - Small Business Professionals</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Interest - Engineering</t>
+  </si>
+  <si>
+    <t>24491</t>
+  </si>
+  <si>
+    <t>1581</t>
+  </si>
+  <si>
+    <t>1583</t>
+  </si>
+  <si>
+    <t>1589</t>
+  </si>
+  <si>
+    <t>Private Client ID</t>
+  </si>
+  <si>
+    <t>Optional
+(Separated by |)</t>
+  </si>
+  <si>
+    <t>1234|4567</t>
+  </si>
 </sst>
 </file>
 
@@ -356,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -504,6 +557,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="34">
@@ -882,7 +941,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -931,6 +990,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1287,13 +1356,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1305,74 +1374,74 @@
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="68">
       <c r="A2" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="21"/>
       <c r="B3">
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1381,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1390,32 +1459,9 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4">
-        <v>20181130001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="3">
-        <v>43412</v>
-      </c>
-      <c r="I4" s="3">
-        <v>43413</v>
-      </c>
+    <row r="5" spans="1:9">
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1424,13 +1470,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -1446,7 +1492,7 @@
     <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1454,10 +1500,10 @@
         <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>28</v>
@@ -1466,7 +1512,7 @@
         <v>41</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>29</v>
@@ -1487,7 +1533,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="119">
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
@@ -1497,8 +1543,8 @@
       <c r="C2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>37</v>
+      <c r="D2" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>37</v>
@@ -1513,42 +1559,42 @@
         <v>37</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>40</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1557,30 +1603,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4">
-        <v>90</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1592,11 +1615,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -1610,7 +1633,7 @@
     <col min="12" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>17</v>
@@ -1645,15 +1668,15 @@
         <v>22</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>33</v>
@@ -1686,13 +1709,13 @@
         <v>36</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>15662758</v>
       </c>
@@ -1700,10 +1723,10 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1730,7 +1753,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>15662759</v>
       </c>
@@ -1738,10 +1761,10 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1777,6 +1800,168 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046AC4F-D72D-9C40-94C8-967158865EC4}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23">
+        <v>1</v>
+      </c>
+      <c r="E3" s="23">
+        <v>1</v>
+      </c>
+      <c r="F3" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1784,12 +1969,12 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="34">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1815,7 +2000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1841,7 +2026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>32048</v>
       </c>
@@ -1864,7 +2049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>31804</v>
       </c>
@@ -1895,21 +2080,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="77.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1919,14 +2105,17 @@
       <c r="C1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>66</v>
+      <c r="D1" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1936,14 +2125,17 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>6</v>
+      <c r="D2" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1111</v>
       </c>
@@ -1954,7 +2146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2222</v>
       </c>
@@ -1963,6 +2155,9 @@
       </c>
       <c r="C4" t="s">
         <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +2165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACD0D70-707D-6848-808A-BFBD2B8DA8BA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1978,25 +2173,25 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="68">
       <c r="A2" s="19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3">
         <v>43405</v>
       </c>

</xml_diff>

<commit_message>
edit custom segment for adobe adcloud is done
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2173B-612D-844A-91A3-1D4497F8630F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E1C1C-D3CB-974D-9C2E-944A1719E928}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="980" windowWidth="31860" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
     <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
-    <sheet name="AppNexus" sheetId="3" r:id="rId3"/>
-    <sheet name="MediaMath" sheetId="8" r:id="rId4"/>
-    <sheet name="TTD" sheetId="1" r:id="rId5"/>
-    <sheet name="Yahoo" sheetId="4" r:id="rId6"/>
-    <sheet name="All Report Platforms" sheetId="7" r:id="rId7"/>
+    <sheet name="Adobe AdCloud" sheetId="9" r:id="rId3"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId4"/>
+    <sheet name="MediaMath" sheetId="8" r:id="rId5"/>
+    <sheet name="TTD" sheetId="1" r:id="rId6"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId7"/>
+    <sheet name="All Report Platforms" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="101">
   <si>
     <t>Segment ID</t>
   </si>
@@ -400,6 +401,32 @@
   </si>
   <si>
     <t>1234|4567</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Test Segment 1</t>
+  </si>
+  <si>
+    <t>Add Custom: Required
+Edit Custom: Required</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>455399-e1ecec9c</t>
+  </si>
+  <si>
+    <t>Eyeota Segment ID</t>
+  </si>
+  <si>
+    <t>Add Custom: Not Required
+Edit Custom: Required</t>
+  </si>
+  <si>
+    <t>AdCloud Segment ID</t>
   </si>
 </sst>
 </file>
@@ -752,7 +779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -895,6 +922,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -941,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -999,6 +1037,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1473,7 +1514,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1612,6 +1653,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689799C4-08DD-4348-87B9-856D4611FF5E}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34">
+      <c r="A2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <v>12345</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.75</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -1799,7 +1937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046AC4F-D72D-9C40-94C8-967158865EC4}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -1961,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2080,11 +2218,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2165,7 +2303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACD0D70-707D-6848-808A-BFBD2B8DA8BA}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
changed sample data in UploadTemplate.xlsx AdobeAAM tab Modelling price to Activation price since we use activation more often
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E1C1C-D3CB-974D-9C2E-944A1719E928}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6207197-20BB-3F4F-9EE4-F4EB31D43953}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1640,10 +1640,10 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689799C4-08DD-4348-87B9-856D4611FF5E}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
completed added and edit custom segments for TTD
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6207197-20BB-3F4F-9EE4-F4EB31D43953}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285DB990-37EF-E543-A817-BA8E1FE8122E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
   <si>
     <t>Segment ID</t>
   </si>
@@ -50,24 +50,6 @@
     <t>Optional</t>
   </si>
   <si>
-    <t>Premium Range Purchasers</t>
-  </si>
-  <si>
-    <t>Users who prefer premium branded ranges over supermarket own brand</t>
-  </si>
-  <si>
-    <t>UK Kantar Media TGI &gt; Grocery Shopping &gt; Premium Range Purchasers</t>
-  </si>
-  <si>
-    <t>TV Channels Watched Live (Last 30 Days)</t>
-  </si>
-  <si>
-    <t>Not Buyable</t>
-  </si>
-  <si>
-    <t>Media &gt; TV And Film &gt; TV Channels Watched Live (Last 30 Days)</t>
-  </si>
-  <si>
     <t>Parent Segment ID</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
   </si>
   <si>
     <t>Just random segment 2222</t>
-  </si>
-  <si>
-    <t>taxoapitest</t>
   </si>
   <si>
     <t>Data Source Name</t>
@@ -427,6 +406,15 @@
   </si>
   <si>
     <t>AdCloud Segment ID</t>
+  </si>
+  <si>
+    <t>ttdratetest_partnerID_rate</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401004</t>
+  </si>
+  <si>
+    <t>fals</t>
   </si>
 </sst>
 </file>
@@ -1420,57 +1408,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68">
       <c r="A2" s="20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1479,10 +1467,10 @@
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1491,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1513,7 +1501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3:M3"/>
     </sheetView>
   </sheetViews>
@@ -1538,104 +1526,104 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="119">
       <c r="A2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="L2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1644,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1671,68 +1659,68 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1776,81 +1764,81 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="L1" s="13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1861,10 +1849,10 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1873,7 +1861,7 @@
         <v>129600</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -1899,10 +1887,10 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1911,7 +1899,7 @@
         <v>129600</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -1960,16 +1948,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>2</v>
@@ -1997,10 +1985,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C3" s="23">
         <v>1</v>
@@ -2019,10 +2007,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2039,10 +2027,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2059,7 +2047,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2076,10 +2064,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2103,12 +2091,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2117,13 +2106,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>2</v>
@@ -2132,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>4</v>
@@ -2166,52 +2155,26 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>32048</v>
+        <v>20190401004</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
+        <v>96</v>
+      </c>
+      <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4">
-        <v>31804</v>
-      </c>
-      <c r="B4">
-        <v>31804</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2241,16 +2204,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34">
@@ -2264,7 +2227,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>6</v>
@@ -2278,10 +2241,10 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2289,13 +2252,13 @@
         <v>2222</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2315,18 +2278,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="68">
       <c r="A2" s="19" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
added Edit Segments for AAM
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285DB990-37EF-E543-A817-BA8E1FE8122E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF1823-CE6A-484D-BB46-D1E1E7F2A8B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="99">
   <si>
     <t>Segment ID</t>
   </si>
@@ -150,28 +150,16 @@
     </r>
   </si>
   <si>
-    <t>Add: Required</t>
-  </si>
-  <si>
     <t>Activation Price</t>
   </si>
   <si>
     <t>Activation UoM</t>
   </si>
   <si>
-    <t>Add: Optional</t>
-  </si>
-  <si>
     <t>Data Feed Description</t>
   </si>
   <si>
-    <t>Add: Optional if data source exists</t>
-  </si>
-  <si>
     <t>Not Required (default FIXED)</t>
-  </si>
-  <si>
-    <t>Add: Optional (FIXED or CPM)</t>
   </si>
   <si>
     <t>CPM</t>
@@ -321,8 +309,95 @@
     <t>/All Traits/3rd-Party Data/test20181207/TEST</t>
   </si>
   <si>
+    <t>uniques</t>
+  </si>
+  <si>
+    <t>Wholesale CPM</t>
+  </si>
+  <si>
+    <t>Retail CPM</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions - Business Owners</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions - C-Suite / C-Level</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions - Small Business Professionals</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Professions</t>
+  </si>
+  <si>
+    <t>Eyeota - Business or B2B - Interest - Engineering</t>
+  </si>
+  <si>
+    <t>24491</t>
+  </si>
+  <si>
+    <t>1581</t>
+  </si>
+  <si>
+    <t>1583</t>
+  </si>
+  <si>
+    <t>1589</t>
+  </si>
+  <si>
+    <t>Private Client ID</t>
+  </si>
+  <si>
+    <t>Optional
+(Separated by |)</t>
+  </si>
+  <si>
+    <t>1234|4567</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Test Segment 1</t>
+  </si>
+  <si>
+    <t>Add Custom: Required
+Edit Custom: Required</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>455399-e1ecec9c</t>
+  </si>
+  <si>
+    <t>Eyeota Segment ID</t>
+  </si>
+  <si>
+    <t>Add Custom: Not Required
+Edit Custom: Required</t>
+  </si>
+  <si>
+    <t>AdCloud Segment ID</t>
+  </si>
+  <si>
+    <t>ttdratetest_partnerID_rate</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401003</t>
+  </si>
+  <si>
+    <t>Add: Not Required
+Edit: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+EditL Required</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Add: Required
+Edit: Required
 </t>
     </r>
     <r>
@@ -336,85 +411,24 @@
     </r>
   </si>
   <si>
-    <t>uniques</t>
-  </si>
-  <si>
-    <t>Wholesale CPM</t>
-  </si>
-  <si>
-    <t>Retail CPM</t>
-  </si>
-  <si>
-    <t>Eyeota - Business or B2B - Professions - Business Owners</t>
-  </si>
-  <si>
-    <t>Eyeota - Business or B2B - Professions - C-Suite / C-Level</t>
-  </si>
-  <si>
-    <t>Eyeota - Business or B2B - Professions - Small Business Professionals</t>
-  </si>
-  <si>
-    <t>Eyeota - Business or B2B - Professions</t>
-  </si>
-  <si>
-    <t>Eyeota - Business or B2B - Interest - Engineering</t>
-  </si>
-  <si>
-    <t>24491</t>
-  </si>
-  <si>
-    <t>1581</t>
-  </si>
-  <si>
-    <t>1583</t>
-  </si>
-  <si>
-    <t>1589</t>
-  </si>
-  <si>
-    <t>Private Client ID</t>
-  </si>
-  <si>
-    <t>Optional
-(Separated by |)</t>
-  </si>
-  <si>
-    <t>1234|4567</t>
-  </si>
-  <si>
-    <t>Lifetime</t>
-  </si>
-  <si>
-    <t>Test Segment 1</t>
-  </si>
-  <si>
-    <t>Add Custom: Required
-Edit Custom: Required</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>455399-e1ecec9c</t>
-  </si>
-  <si>
-    <t>Eyeota Segment ID</t>
-  </si>
-  <si>
-    <t>Add Custom: Not Required
-Edit Custom: Required</t>
-  </si>
-  <si>
-    <t>AdCloud Segment ID</t>
-  </si>
-  <si>
-    <t>ttdratetest_partnerID_rate</t>
-  </si>
-  <si>
-    <t>Test Segment 20190401004</t>
-  </si>
-  <si>
-    <t>fals</t>
+    <t>Add: Optional if data source exists
+Edit: Not required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Optional
+Edit: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Optional (FIXED or CPM)
+Edit: Not Required</t>
   </si>
 </sst>
 </file>
@@ -967,7 +981,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -992,9 +1006,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1029,6 +1040,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1404,73 +1419,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68">
-      <c r="A2" s="20" t="s">
-        <v>56</v>
+      <c r="A2" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="21"/>
+      <c r="A3" s="20"/>
       <c r="B3">
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1479,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1489,8 +1504,8 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1499,140 +1514,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:M3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="136">
+      <c r="A2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
         <v>34</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="119">
-      <c r="A2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>90</v>
-      </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1659,10 +1681,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1671,56 +1693,56 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>93</v>
+        <v>81</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1760,49 +1782,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>42</v>
+      <c r="L1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>66</v>
+      <c r="A2" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -1831,14 +1853,14 @@
       <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>52</v>
+      <c r="L2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1849,10 +1871,10 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1887,10 +1909,10 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1944,22 +1966,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1985,32 +2007,32 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <v>1</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>1</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>1</v>
       </c>
-      <c r="F3" s="24" t="b">
+      <c r="F3" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2021,16 +2043,16 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="24" t="b">
+      <c r="F4" s="23" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2041,13 +2063,13 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" s="24" t="b">
+      <c r="F5" s="23" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2058,16 +2080,16 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" s="25" t="b">
+      <c r="F6" s="24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2078,7 +2100,7 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="25" t="b">
+      <c r="F7" s="24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2091,39 +2113,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="A10:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2143,34 +2164,31 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>20190401004</v>
+        <v>20190401003</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2197,23 +2215,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>55</v>
+      <c r="D1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34">
@@ -2227,12 +2245,12 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2258,7 +2276,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2277,19 +2295,19 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>42</v>
+      <c r="A1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="68">
-      <c r="A2" s="19" t="s">
-        <v>43</v>
+      <c r="A2" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
changed edit required for data category and data type
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF1823-CE6A-484D-BB46-D1E1E7F2A8B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6475175-1E3E-9947-A227-F1773BF5DA39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -1516,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1763,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1848,10 +1848,10 @@
         <v>28</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
changed data segment type id to data segment type
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6475175-1E3E-9947-A227-F1773BF5DA39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A98461-7345-164E-82E3-78EE70B9F54F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
   <si>
     <t>Segment ID</t>
   </si>
@@ -228,9 +228,6 @@
     </r>
   </si>
   <si>
-    <t>Data Segment Type ID</t>
-  </si>
-  <si>
     <t>Segment Key</t>
   </si>
   <si>
@@ -429,6 +426,15 @@
   <si>
     <t>Add: Optional (FIXED or CPM)
 Edit: Not Required</t>
+  </si>
+  <si>
+    <t>Data Segment Type</t>
+  </si>
+  <si>
+    <t>B2B</t>
+  </si>
+  <si>
+    <t>In-Market</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1444,7 @@
         <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>37</v>
@@ -1449,25 +1455,25 @@
     </row>
     <row r="2" spans="1:9" ht="68">
       <c r="A2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1482,7 +1488,7 @@
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -1494,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1560,7 +1566,7 @@
         <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>22</v>
@@ -1583,46 +1589,46 @@
     </row>
     <row r="2" spans="1:14" ht="136">
       <c r="A2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>96</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="M2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1636,16 +1642,16 @@
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1681,10 +1687,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1693,53 +1699,53 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1764,7 +1770,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1807,7 +1813,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>11</v>
@@ -1824,7 +1830,7 @@
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -1871,7 +1877,7 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1888,8 +1894,8 @@
       <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="I3">
-        <v>100</v>
+      <c r="I3" t="s">
+        <v>99</v>
       </c>
       <c r="J3">
         <v>4299</v>
@@ -1909,7 +1915,7 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -1926,8 +1932,8 @@
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>200</v>
+      <c r="I4" t="s">
+        <v>100</v>
       </c>
       <c r="J4">
         <v>4299</v>
@@ -1973,13 +1979,13 @@
         <v>9</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>2</v>
@@ -2007,10 +2013,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="22">
         <v>1</v>
@@ -2029,10 +2035,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2049,10 +2055,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2069,7 +2075,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2086,10 +2092,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2179,13 +2185,13 @@
         <v>20190401003</v>
       </c>
       <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -2225,13 +2231,13 @@
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34">
@@ -2245,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>6</v>
@@ -2276,7 +2282,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rates api for ttd
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A98461-7345-164E-82E3-78EE70B9F54F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E402105-8723-1243-8808-8911031FD57F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1640" windowWidth="24320" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="111">
   <si>
     <t>Segment ID</t>
   </si>
@@ -435,6 +435,52 @@
   </si>
   <si>
     <t>In-Market</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>bombora</t>
+  </si>
+  <si>
+    <t>Seat ID</t>
+  </si>
+  <si>
+    <t>Batch ID</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required
+"bombora" or "eyeota" only</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required</t>
+  </si>
+  <si>
+    <t>Add/Edit: Optional
+Edit Rates: Optional
+Retrieve Batch: Required
+Retrieve Rates: Optional</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1033,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1024,7 +1070,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1050,6 +1095,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1454,7 +1505,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="68">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1483,7 +1534,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3">
         <v>20181130001</v>
       </c>
@@ -1510,8 +1561,8 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1544,7 +1595,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1588,7 +1639,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="136">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1707,7 +1758,7 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1769,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -2018,20 +2069,20 @@
       <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>1</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>1</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>1</v>
       </c>
-      <c r="F3" s="23" t="b">
+      <c r="F3" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -2049,7 +2100,7 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="23" t="b">
+      <c r="F4" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2069,7 +2120,7 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" s="23" t="b">
+      <c r="F5" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2086,7 +2137,7 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" s="24" t="b">
+      <c r="F6" s="23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2106,7 +2157,7 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="24" t="b">
+      <c r="F7" s="23" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2117,18 +2168,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="A10:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="8" max="8" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2145,42 +2203,60 @@
         <v>2</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="16" t="s">
+    <row r="2" spans="1:11" ht="85">
+      <c r="A2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="K2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>20190401003</v>
       </c>
@@ -2196,9 +2272,22 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="G4" s="1"/>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3">
+        <v>1.25</v>
+      </c>
+      <c r="I3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2253,10 +2342,10 @@
       <c r="D2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2309,7 +2398,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="68">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="10" t="s">

</xml_diff>

<commit_message>
added delete function for adform
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E402105-8723-1243-8808-8911031FD57F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBF91C-4C74-CC40-B74E-94761181F2EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="112">
   <si>
     <t>Segment ID</t>
   </si>
@@ -234,18 +234,8 @@
     <t>Eyeota Segment Name</t>
   </si>
   <si>
-    <t>Add: Not required
-Edit: Required</t>
-  </si>
-  <si>
     <t>Add: Required
 Edit: Required</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
-Values: global, apac
-Defaulted to global</t>
   </si>
   <si>
     <t>Distribution</t>
@@ -481,6 +471,23 @@
 Edit Rates: Optional
 Retrieve Batch: Required
 Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Not required
+Edit: Required
+Delete: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required
+Values: global, apac
+Defaulted to global</t>
   </si>
 </sst>
 </file>
@@ -1459,18 +1466,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1495,7 +1502,7 @@
         <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>37</v>
@@ -1504,27 +1511,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="68">
+    <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1539,7 +1546,7 @@
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -1551,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1617,7 +1624,7 @@
         <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>22</v>
@@ -1640,46 +1647,46 @@
     </row>
     <row r="2" spans="1:14" ht="136">
       <c r="A2" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1693,16 +1700,16 @@
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1738,10 +1745,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1750,53 +1757,53 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1864,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>11</v>
@@ -1881,7 +1888,7 @@
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -1928,7 +1935,7 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -1946,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J3">
         <v>4299</v>
@@ -1966,7 +1973,7 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -1984,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J4">
         <v>4299</v>
@@ -2030,13 +2037,13 @@
         <v>9</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>2</v>
@@ -2064,10 +2071,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="21">
         <v>1</v>
@@ -2086,10 +2093,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2106,10 +2113,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2126,7 +2133,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2143,10 +2150,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2170,7 +2177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -2203,16 +2210,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>3</v>
@@ -2223,31 +2230,31 @@
     </row>
     <row r="2" spans="1:11" ht="85">
       <c r="A2" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="H2" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>110</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>6</v>
@@ -2261,22 +2268,22 @@
         <v>20190401003</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3">
         <v>1.25</v>
@@ -2320,7 +2327,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>49</v>
@@ -2340,7 +2347,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>6</v>
@@ -2371,7 +2378,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added price type to accommodate percentage media for TTD
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBF91C-4C74-CC40-B74E-94761181F2EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BCD870-A890-664B-AD77-46376FD2653E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
   <si>
     <t>Segment ID</t>
   </si>
@@ -488,6 +488,25 @@
 Delete: Not Required
 Values: global, apac
 Defaulted to global</t>
+  </si>
+  <si>
+    <t>Price Type</t>
+  </si>
+  <si>
+    <t>Add/Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional
+Values: CPM or PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>eyeota</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401004</t>
   </si>
 </sst>
 </file>
@@ -1466,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2175,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2189,11 +2208,12 @@
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" customWidth="1"/>
     <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17">
+    <row r="1" spans="1:12" ht="17">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2219,16 +2239,19 @@
         <v>13</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="85">
+    <row r="2" spans="1:12" ht="102">
       <c r="A2" s="27" t="s">
         <v>104</v>
       </c>
@@ -2254,16 +2277,19 @@
         <v>104</v>
       </c>
       <c r="I2" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>6</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>20190401003</v>
       </c>
@@ -2288,13 +2314,44 @@
       <c r="H3">
         <v>1.25</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>20190401004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4">
+        <v>23456</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added get uniques for AAM'
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BCD870-A890-664B-AD77-46376FD2653E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9ABE0F-37D7-A344-BBED-E824829C7429}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
   <si>
     <t>Segment ID</t>
   </si>
@@ -507,6 +507,11 @@
   </si>
   <si>
     <t>Test Segment 20190401004</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Get Uniques: Required</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1609,7 +1614,7 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
     <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
@@ -1681,7 +1686,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2196,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C7:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
edited UploadTemplate TTD Add and Edit requirement separated
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9ABE0F-37D7-A344-BBED-E824829C7429}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7563D9E6-2CF8-7A47-A152-4AC8468B917A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
   <si>
     <t>Segment ID</t>
   </si>
@@ -442,37 +442,6 @@
     <t>Batch ID</t>
   </si>
   <si>
-    <t>Add/Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
-    <t>Add/Edit: Required
-Edit Rates: Optional
-Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
-    <t>Add/Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Required
-"bombora" or "eyeota" only</t>
-  </si>
-  <si>
-    <t>Add/Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Required</t>
-  </si>
-  <si>
-    <t>Add/Edit: Optional
-Edit Rates: Optional
-Retrieve Batch: Required
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
     <t>Add: Not required
 Edit: Required
 Delete: Required</t>
@@ -493,25 +462,69 @@
     <t>Price Type</t>
   </si>
   <si>
-    <t>Add/Edit: Required
+    <t>PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>eyeota</t>
+  </si>
+  <si>
+    <t>Test Segment 20190401004</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Get Uniques: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required
+"bombora" or "eyeota" only</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Required</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Rates: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
 Retrieve Rates: Optional
 Values: CPM or PercentOfMediaCost</t>
   </si>
   <si>
-    <t>PercentOfMediaCost</t>
-  </si>
-  <si>
-    <t>eyeota</t>
-  </si>
-  <si>
-    <t>Test Segment 20190401004</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
-Get Uniques: Required</t>
+    <t>Add: Not Required
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Required
+Retrieve Rates: Optional</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1077,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,6 +1144,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1537,25 +1553,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1604,7 +1620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1686,7 +1702,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2201,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:M8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2244,7 +2260,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>103</v>
@@ -2256,36 +2272,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="102">
+    <row r="2" spans="1:12" ht="119">
       <c r="A2" s="27" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>108</v>
+        <v>117</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>6</v>
@@ -2334,16 +2350,16 @@
         <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
         <v>100</v>
@@ -2352,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J4">
         <v>23456</v>

</xml_diff>

<commit_message>
added rates to query all and retrieve custom segments
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7563D9E6-2CF8-7A47-A152-4AC8468B917A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C361F1-26FD-2644-9190-EE37FDE87A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,53 +478,53 @@
   <si>
     <t>Add: Required
 Edit: Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Required
 Edit Rates: Optional
 Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
+Retrieve Custom: Optional</t>
   </si>
   <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
-Retrieve Rates: Required
-"bombora" or "eyeota" only</t>
+Retrieve Custom: Required</t>
   </si>
   <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
-Retrieve Rates: Required</t>
+Retrieve Custom: Optional</t>
   </si>
   <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
-Retrieve Rates: Optional</t>
+Retrieve Custom: Optional
+Values: CPM or PercentOfMediaCost</t>
+  </si>
+  <si>
+    <t>Add: Not Required
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Required
+Retrieve Custom: Optional</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Edit Rates: Required
+Retrieve Batch: Optional
+Retrieve Custom: Required</t>
   </si>
   <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
-Retrieve Rates: Optional
-Values: CPM or PercentOfMediaCost</t>
-  </si>
-  <si>
-    <t>Add: Not Required
-Edit: Not Required
-Edit Rates: Optional
-Retrieve Batch: Required
-Retrieve Rates: Optional</t>
+Retrieve Custom: Optional
+"bombora" or "eyeota" only</t>
   </si>
 </sst>
 </file>
@@ -2217,20 +2217,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.83203125" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2274,34 +2273,34 @@
     </row>
     <row r="2" spans="1:12" ht="119">
       <c r="A2" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="H2" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="J2" s="29" t="s">
         <v>116</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>118</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
changed TTD advertiser ID to do not use
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C361F1-26FD-2644-9190-EE37FDE87A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6453E9-D164-7242-B4B3-473BBEA61215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
   <si>
     <t>Segment ID</t>
   </si>
@@ -436,9 +436,6 @@
     <t>bombora</t>
   </si>
   <si>
-    <t>Seat ID</t>
-  </si>
-  <si>
     <t>Batch ID</t>
   </si>
   <si>
@@ -481,13 +478,6 @@
 Edit Rates: Optional
 Retrieve Batch: Optional
 Retrieve Custom: Optional</t>
-  </si>
-  <si>
-    <t>Add: Required
-Edit: Not Required
-Edit Rates: Required
-Retrieve Batch: Optional
-Retrieve Custom: Required</t>
   </si>
   <si>
     <t>Add: Required
@@ -525,6 +515,25 @@
 Retrieve Batch: Optional
 Retrieve Custom: Optional
 "bombora" or "eyeota" only</t>
+  </si>
+  <si>
+    <t>Partner ID</t>
+  </si>
+  <si>
+    <t>Add: Optional
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Custom: Required</t>
+  </si>
+  <si>
+    <t>Advertiser ID</t>
+  </si>
+  <si>
+    <t>def456</t>
+  </si>
+  <si>
+    <t>Do not use!!</t>
   </si>
 </sst>
 </file>
@@ -690,7 +699,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -873,6 +882,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,7 +1092,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1146,6 +1161,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1553,25 +1571,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1702,7 +1720,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2215,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2227,13 +2245,13 @@
     <col min="2" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.83203125" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="8" width="23.83203125" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="7" max="9" width="23.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17">
+    <row r="1" spans="1:13" ht="17">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2253,63 +2271,69 @@
         <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="119">
+    <row r="2" spans="1:13" ht="119">
       <c r="A2" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>114</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>6</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>20190401003</v>
       </c>
@@ -2331,17 +2355,20 @@
       <c r="G3" t="s">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3">
         <v>1.25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>34</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>20190401004</v>
       </c>
@@ -2349,27 +2376,30 @@
         <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" t="s">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4">
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4">
         <v>23456</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edited brand id for ttd
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/Local/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6453E9-D164-7242-B4B3-473BBEA61215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD10A92F-090F-5741-A09E-A49E4EFF80B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,31 +509,31 @@
 Retrieve Custom: Required</t>
   </si>
   <si>
+    <t>Partner ID</t>
+  </si>
+  <si>
+    <t>Add: Optional
+Edit: Not Required
+Edit Rates: Optional
+Retrieve Batch: Optional
+Retrieve Custom: Required</t>
+  </si>
+  <si>
+    <t>Advertiser ID</t>
+  </si>
+  <si>
+    <t>def456</t>
+  </si>
+  <si>
+    <t>Do not use!!</t>
+  </si>
+  <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
 Retrieve Custom: Optional
-"bombora" or "eyeota" only</t>
-  </si>
-  <si>
-    <t>Partner ID</t>
-  </si>
-  <si>
-    <t>Add: Optional
-Edit: Not Required
-Edit Rates: Optional
-Retrieve Batch: Optional
-Retrieve Custom: Required</t>
-  </si>
-  <si>
-    <t>Advertiser ID</t>
-  </si>
-  <si>
-    <t>def456</t>
-  </si>
-  <si>
-    <t>Do not use!!</t>
+"bombora" or "eyeota" or fill in the Brand ID</t>
   </si>
 </sst>
 </file>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2271,10 +2271,10 @@
         <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>13</v>
@@ -2309,13 +2309,13 @@
         <v>111</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>112</v>
@@ -2356,7 +2356,7 @@
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -2391,7 +2391,7 @@
         <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4">
         <v>1</v>

</xml_diff>

<commit_message>
changed fake partner id for ttd
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/PROD/prodplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/Local/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD10A92F-090F-5741-A09E-A49E4EFF80B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7651765-066D-8D44-96CD-67033F2EB97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,9 +430,6 @@
     <t>Brand</t>
   </si>
   <si>
-    <t>abc123</t>
-  </si>
-  <si>
     <t>bombora</t>
   </si>
   <si>
@@ -534,6 +531,9 @@
 Retrieve Batch: Optional
 Retrieve Custom: Optional
 "bombora" or "eyeota" or fill in the Brand ID</t>
+  </si>
+  <si>
+    <t>7s3xqae</t>
   </si>
 </sst>
 </file>
@@ -1571,25 +1571,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1720,7 +1720,7 @@
         <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>91</v>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2271,19 +2271,19 @@
         <v>99</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>3</v>
@@ -2294,37 +2294,37 @@
     </row>
     <row r="2" spans="1:13" ht="119">
       <c r="A2" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>113</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>114</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>6</v>
@@ -2350,13 +2350,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -2376,28 +2376,28 @@
         <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K4">
         <v>23456</v>

</xml_diff>

<commit_message>
change brand to be mandatory for retrieve custom segment
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/Local/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7651765-066D-8D44-96CD-67033F2EB97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90085974-C033-8642-B387-BA291BD6CC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,15 +525,15 @@
     <t>Do not use!!</t>
   </si>
   <si>
+    <t>7s3xqae</t>
+  </si>
+  <si>
     <t>Add: Required
 Edit: Not Required
 Edit Rates: Required
 Retrieve Batch: Optional
-Retrieve Custom: Optional
+Retrieve Custom: Required
 "bombora" or "eyeota" or fill in the Brand ID</t>
-  </si>
-  <si>
-    <t>7s3xqae</t>
   </si>
 </sst>
 </file>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2309,7 +2309,7 @@
         <v>110</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>116</v>
@@ -2353,7 +2353,7 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" t="s">
         <v>118</v>
@@ -2388,7 +2388,7 @@
         <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
streamlined adform for new accounts, changed Region to Account in UploadTemplate
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90085974-C033-8642-B387-BA291BD6CC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6EC836-C308-6841-AB1A-73FDB8E3FF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="121">
   <si>
     <t>Segment ID</t>
   </si>
@@ -189,9 +189,6 @@
     <t>TTL</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
     <t>apac</t>
   </si>
   <si>
@@ -446,13 +443,6 @@
 Delete: Not Required</t>
   </si>
   <si>
-    <t>Add: Required
-Edit: Required
-Delete: Not Required
-Values: global, apac
-Defaulted to global</t>
-  </si>
-  <si>
     <t>Price Type</t>
   </si>
   <si>
@@ -534,6 +524,13 @@
 Retrieve Batch: Optional
 Retrieve Custom: Required
 "bombora" or "eyeota" or fill in the Brand ID</t>
+  </si>
+  <si>
+    <t>Add: Required
+Edit: Required
+Delete: Not Required
+Values: global, apac, mastercard, experian
+Defaulted to global</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1551,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>41</v>
@@ -1560,7 +1557,7 @@
         <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>37</v>
@@ -1571,31 +1568,31 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1604,10 +1601,10 @@
         <v>20181130001</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1616,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="3">
         <v>43405</v>
@@ -1682,7 +1679,7 @@
         <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>22</v>
@@ -1705,69 +1702,69 @@
     </row>
     <row r="2" spans="1:14" ht="136">
       <c r="A2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="M2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1803,10 +1800,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1815,56 +1812,56 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34">
       <c r="A2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <v>12345</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1929,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>11</v>
@@ -1946,7 +1943,7 @@
     </row>
     <row r="2" spans="1:13" ht="68" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -1982,7 +1979,7 @@
         <v>39</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1993,10 +1990,10 @@
         <v>-2018113011</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -2011,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J3">
         <v>4299</v>
@@ -2031,10 +2028,10 @@
         <v>-2018113012</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -2049,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J4">
         <v>4299</v>
@@ -2095,13 +2092,13 @@
         <v>9</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>2</v>
@@ -2129,10 +2126,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="21">
         <v>1</v>
@@ -2151,10 +2148,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2171,10 +2168,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2191,7 +2188,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2208,10 +2205,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2235,7 +2232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2268,22 +2265,22 @@
         <v>2</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>117</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>3</v>
@@ -2294,37 +2291,37 @@
     </row>
     <row r="2" spans="1:13" ht="119">
       <c r="A2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="H2" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>113</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>6</v>
@@ -2338,25 +2335,25 @@
         <v>20190401003</v>
       </c>
       <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -2373,31 +2370,31 @@
         <v>20190401004</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K4">
         <v>23456</v>
@@ -2434,13 +2431,13 @@
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34">
@@ -2454,7 +2451,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>6</v>
@@ -2485,7 +2482,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2516,7 +2513,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
added delete segments function for AAM
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6EC836-C308-6841-AB1A-73FDB8E3FF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10276F2-6996-8342-9DE7-2FD41C638184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="120">
   <si>
     <t>Segment ID</t>
   </si>
@@ -371,14 +371,6 @@
     <t>Test Segment 20190401003</t>
   </si>
   <si>
-    <t>Add: Not Required
-Edit: Required</t>
-  </si>
-  <si>
-    <t>Add: Required
-EditL Required</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Add: Required
 Edit: Required
@@ -531,6 +523,11 @@
 Delete: Not Required
 Values: global, apac, mastercard, experian
 Defaulted to global</t>
+  </si>
+  <si>
+    <t>Add: Not Required
+Edit: Required
+Delete: Required</t>
   </si>
 </sst>
 </file>
@@ -1521,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DE401A-9862-6C4F-BF9F-D68D31DB6CEF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1568,25 +1565,25 @@
     </row>
     <row r="2" spans="1:9" ht="82" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>39</v>
@@ -1635,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1702,10 +1699,10 @@
     </row>
     <row r="2" spans="1:14" ht="136">
       <c r="A2" s="25" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>50</v>
@@ -1714,34 +1711,34 @@
         <v>50</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1926,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>11</v>
@@ -2008,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J3">
         <v>4299</v>
@@ -2046,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J4">
         <v>4299</v>
@@ -2265,22 +2262,22 @@
         <v>2</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>3</v>
@@ -2291,37 +2288,37 @@
     </row>
     <row r="2" spans="1:13" ht="119">
       <c r="A2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="H2" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>111</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>6</v>
@@ -2347,13 +2344,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I3">
         <v>1.25</v>
@@ -2373,28 +2370,28 @@
         <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K4">
         <v>23456</v>

</xml_diff>

<commit_message>
Add Amazon API part 1
</commit_message>
<xml_diff>
--- a/UploadTemplate.xlsx
+++ b/UploadTemplate.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Data Ops/Heroku/localplatformsapp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasminekoh/Documents/API APPLICATION/localplatformsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10276F2-6996-8342-9DE7-2FD41C638184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27B570-8CEE-E44D-B512-4D0A2F371DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2040" windowWidth="29360" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="460" windowWidth="29360" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adform" sheetId="6" r:id="rId1"/>
     <sheet name="Adobe AAM" sheetId="5" r:id="rId2"/>
     <sheet name="Adobe AdCloud" sheetId="9" r:id="rId3"/>
-    <sheet name="AppNexus" sheetId="3" r:id="rId4"/>
-    <sheet name="MediaMath" sheetId="8" r:id="rId5"/>
-    <sheet name="TTD" sheetId="1" r:id="rId6"/>
-    <sheet name="Yahoo" sheetId="4" r:id="rId7"/>
-    <sheet name="All Report Platforms" sheetId="7" r:id="rId8"/>
+    <sheet name="Amazon" sheetId="10" r:id="rId4"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId5"/>
+    <sheet name="MediaMath" sheetId="8" r:id="rId6"/>
+    <sheet name="TTD" sheetId="1" r:id="rId7"/>
+    <sheet name="Yahoo" sheetId="4" r:id="rId8"/>
+    <sheet name="All Report Platforms" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="127">
   <si>
     <t>Segment ID</t>
   </si>
@@ -528,6 +529,36 @@
     <t>Add: Not Required
 Edit: Required
 Delete: Required</t>
+  </si>
+  <si>
+    <t>Amazon ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add: Not Required
+Edit: Required
+Retrieve: Required
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add: Required
+Edit: Not Required
+Retrieve: Not Required
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add: Required
+Edit: Required
+Retrieve: Not Required
+</t>
+  </si>
+  <si>
+    <t>id='426078747047397868'</t>
+  </si>
+  <si>
+    <t>Eyeota Test Segment_11June_mobile</t>
+  </si>
+  <si>
+    <t>This is a test segment for Amazon JP Advertiser, created on 11th June. Test edit description.</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1117,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1160,6 +1191,8 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1632,7 +1665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1876,6 +1909,99 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70808106-77DC-014F-AA2E-F903F6273321}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="34">
+      <c r="A1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="153">
+      <c r="A2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3">
+        <v>-2147269415</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>2592000</v>
+      </c>
+      <c r="G3" s="32">
+        <v>6259435010103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -2063,7 +2189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046AC4F-D72D-9C40-94C8-967158865EC4}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -2225,7 +2351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -2402,7 +2528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2487,7 +2613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACD0D70-707D-6848-808A-BFBD2B8DA8BA}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>